<commit_message>
se cambiaron los porcentajes del Cronograma del proyecto (SACNS-DCP) y se corrigio un error en el nombre de un item(SIN MODIFICAR NINGUNA FECHA)
</commit_message>
<xml_diff>
--- a/Desarrollo/SACNS/gestion/SACNS-DCP.xlsx
+++ b/Desarrollo/SACNS/gestion/SACNS-DCP.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="102">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="105">
   <si>
     <t>CRONOGRAMA DEL PROYECTO</t>
   </si>
@@ -80,7 +80,7 @@
     <t>Desarrollo del Cronograma de Proyecto</t>
   </si>
   <si>
-    <t>Plan de Proyecto(Cronograma del proyecto)</t>
+    <t>Docuemento de cronograma del proyecto</t>
   </si>
   <si>
     <t>SACNS-DCP.XLSX</t>
@@ -99,6 +99,15 @@
   </si>
   <si>
     <t>Llerena/DF,Araujo/SM,Lazaro A /SM,Ramos /JP / DF</t>
+  </si>
+  <si>
+    <t>Plan del proyecto</t>
+  </si>
+  <si>
+    <t>Documento del plan de proyecto</t>
+  </si>
+  <si>
+    <t>SACNS-DPP-DOCX</t>
   </si>
   <si>
     <t xml:space="preserve"> </t>
@@ -329,7 +338,7 @@
     <numFmt numFmtId="165" formatCode="dd&quot;/&quot;mm&quot;/&quot;yyyy"/>
     <numFmt numFmtId="166" formatCode="dd/mm/yyyy"/>
   </numFmts>
-  <fonts count="8">
+  <fonts count="9">
     <font>
       <sz val="11.0"/>
       <color theme="1"/>
@@ -354,6 +363,10 @@
     </font>
     <font>
       <color theme="1"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11.0"/>
       <name val="Calibri"/>
     </font>
     <font>
@@ -442,7 +455,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="32">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -484,10 +497,13 @@
     <xf borderId="1" fillId="0" fontId="2" numFmtId="9" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment readingOrder="0"/>
     </xf>
+    <xf borderId="1" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
     <xf borderId="1" fillId="0" fontId="2" numFmtId="166" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment readingOrder="0"/>
     </xf>
-    <xf borderId="1" fillId="2" fontId="5" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="1" fillId="2" fontId="6" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
     <xf borderId="1" fillId="2" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
     <xf borderId="1" fillId="2" fontId="2" numFmtId="165" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment readingOrder="0"/>
@@ -504,16 +520,16 @@
     <xf borderId="1" fillId="2" fontId="2" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment readingOrder="0"/>
     </xf>
-    <xf borderId="1" fillId="5" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
+    <xf borderId="1" fillId="5" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf borderId="1" fillId="6" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
+    <xf borderId="1" fillId="6" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
-    <xf borderId="1" fillId="0" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="1" fillId="0" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
-    <xf borderId="2" fillId="0" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="2" fillId="0" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
     <xf borderId="2" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
@@ -910,43 +926,44 @@
       </c>
     </row>
     <row r="13" ht="19.5" customHeight="1">
-      <c r="A13" s="2" t="s">
+      <c r="A13" s="2"/>
+      <c r="B13" s="17" t="s">
         <v>29</v>
       </c>
-      <c r="B13" s="13" t="s">
+      <c r="C13" s="17" t="s">
         <v>30</v>
       </c>
-      <c r="C13" s="13" t="s">
+      <c r="D13" s="14" t="s">
         <v>31</v>
       </c>
-      <c r="D13" s="14" t="s">
-        <v>32</v>
-      </c>
       <c r="E13" s="14" t="s">
-        <v>33</v>
+        <v>24</v>
       </c>
       <c r="F13" s="15">
+        <v>44480.0</v>
+      </c>
+      <c r="G13" s="15">
         <v>44487.0</v>
-      </c>
-      <c r="G13" s="15">
-        <v>44494.0</v>
       </c>
       <c r="H13" s="16">
         <v>1.0</v>
       </c>
     </row>
     <row r="14" ht="19.5" customHeight="1">
+      <c r="A14" s="2" t="s">
+        <v>32</v>
+      </c>
       <c r="B14" s="13" t="s">
+        <v>33</v>
+      </c>
+      <c r="C14" s="13" t="s">
         <v>34</v>
       </c>
-      <c r="C14" s="13" t="s">
+      <c r="D14" s="14" t="s">
         <v>35</v>
       </c>
-      <c r="D14" s="14" t="s">
+      <c r="E14" s="14" t="s">
         <v>36</v>
-      </c>
-      <c r="E14" s="14" t="s">
-        <v>37</v>
       </c>
       <c r="F14" s="15">
         <v>44487.0</v>
@@ -960,16 +977,16 @@
     </row>
     <row r="15" ht="19.5" customHeight="1">
       <c r="B15" s="13" t="s">
+        <v>37</v>
+      </c>
+      <c r="C15" s="13" t="s">
         <v>38</v>
       </c>
-      <c r="C15" s="13" t="s">
+      <c r="D15" s="14" t="s">
         <v>39</v>
       </c>
-      <c r="D15" s="14" t="s">
+      <c r="E15" s="14" t="s">
         <v>40</v>
-      </c>
-      <c r="E15" s="14" t="s">
-        <v>41</v>
       </c>
       <c r="F15" s="15">
         <v>44487.0</v>
@@ -983,16 +1000,16 @@
     </row>
     <row r="16" ht="19.5" customHeight="1">
       <c r="B16" s="13" t="s">
+        <v>41</v>
+      </c>
+      <c r="C16" s="13" t="s">
         <v>42</v>
       </c>
-      <c r="C16" s="13" t="s">
+      <c r="D16" s="14" t="s">
         <v>43</v>
       </c>
-      <c r="D16" s="14" t="s">
+      <c r="E16" s="14" t="s">
         <v>44</v>
-      </c>
-      <c r="E16" s="14" t="s">
-        <v>45</v>
       </c>
       <c r="F16" s="15">
         <v>44487.0</v>
@@ -1005,192 +1022,192 @@
       </c>
     </row>
     <row r="17" ht="19.5" customHeight="1">
-      <c r="B17" s="14" t="s">
+      <c r="B17" s="13" t="s">
+        <v>45</v>
+      </c>
+      <c r="C17" s="13" t="s">
         <v>46</v>
       </c>
-      <c r="C17" s="13" t="s">
+      <c r="D17" s="14" t="s">
         <v>47</v>
       </c>
-      <c r="D17" s="14" t="s">
+      <c r="E17" s="14" t="s">
         <v>48</v>
       </c>
-      <c r="E17" s="14" t="s">
-        <v>49</v>
-      </c>
       <c r="F17" s="15">
-        <v>44493.0</v>
+        <v>44487.0</v>
       </c>
       <c r="G17" s="15">
-        <v>44500.0</v>
+        <v>44494.0</v>
       </c>
       <c r="H17" s="16">
         <v>1.0</v>
       </c>
     </row>
     <row r="18" ht="19.5" customHeight="1">
-      <c r="B18" s="13" t="s">
+      <c r="B18" s="14" t="s">
+        <v>49</v>
+      </c>
+      <c r="C18" s="13" t="s">
         <v>50</v>
       </c>
-      <c r="C18" s="13" t="s">
-        <v>19</v>
-      </c>
-      <c r="D18" s="13" t="s">
-        <v>19</v>
-      </c>
-      <c r="E18" s="13"/>
+      <c r="D18" s="14" t="s">
+        <v>51</v>
+      </c>
+      <c r="E18" s="14" t="s">
+        <v>52</v>
+      </c>
       <c r="F18" s="15">
-        <v>44501.0</v>
-      </c>
-      <c r="G18" s="17">
-        <v>44501.0</v>
+        <v>44493.0</v>
+      </c>
+      <c r="G18" s="15">
+        <v>44500.0</v>
       </c>
       <c r="H18" s="16">
         <v>1.0</v>
       </c>
     </row>
     <row r="19" ht="19.5" customHeight="1">
-      <c r="B19" s="18" t="s">
-        <v>51</v>
-      </c>
-      <c r="C19" s="19"/>
-      <c r="D19" s="19"/>
-      <c r="E19" s="19"/>
-      <c r="F19" s="20">
+      <c r="B19" s="13" t="s">
+        <v>53</v>
+      </c>
+      <c r="C19" s="13" t="s">
+        <v>19</v>
+      </c>
+      <c r="D19" s="13" t="s">
+        <v>19</v>
+      </c>
+      <c r="E19" s="13"/>
+      <c r="F19" s="15">
+        <v>44501.0</v>
+      </c>
+      <c r="G19" s="18">
+        <v>44501.0</v>
+      </c>
+      <c r="H19" s="16">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="20" ht="19.5" customHeight="1">
+      <c r="B20" s="19" t="s">
+        <v>54</v>
+      </c>
+      <c r="C20" s="20"/>
+      <c r="D20" s="20"/>
+      <c r="E20" s="20"/>
+      <c r="F20" s="21">
         <v>44480.0</v>
       </c>
-      <c r="G19" s="20">
+      <c r="G20" s="21">
         <v>44501.0</v>
       </c>
-      <c r="H19" s="21">
-        <f>(H10+H11+H12+H13+H14+H15+H16+H17+H18)/9</f>
+      <c r="H20" s="22">
+        <f>(H10+H11+H12+H14+H15+H16+H17+H18+H19)/9</f>
         <v>1</v>
       </c>
     </row>
-    <row r="20" ht="19.5" customHeight="1">
-      <c r="B20" s="13" t="s">
-        <v>52</v>
-      </c>
-      <c r="C20" s="13" t="s">
+    <row r="21" ht="19.5" customHeight="1">
+      <c r="B21" s="13" t="s">
+        <v>55</v>
+      </c>
+      <c r="C21" s="13" t="s">
+        <v>56</v>
+      </c>
+      <c r="D21" s="14" t="s">
+        <v>57</v>
+      </c>
+      <c r="E21" s="14" t="s">
+        <v>58</v>
+      </c>
+      <c r="F21" s="18">
+        <v>44501.0</v>
+      </c>
+      <c r="G21" s="18">
+        <v>44514.0</v>
+      </c>
+      <c r="H21" s="16">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="22" ht="19.5" customHeight="1">
+      <c r="B22" s="23" t="s">
+        <v>59</v>
+      </c>
+      <c r="C22" s="14" t="s">
+        <v>60</v>
+      </c>
+      <c r="D22" s="14" t="s">
+        <v>61</v>
+      </c>
+      <c r="E22" s="14" t="s">
+        <v>62</v>
+      </c>
+      <c r="F22" s="18">
+        <v>44501.0</v>
+      </c>
+      <c r="G22" s="18">
+        <v>44521.0</v>
+      </c>
+      <c r="H22" s="16">
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="23" ht="19.5" customHeight="1">
+      <c r="B23" s="13" t="s">
         <v>53</v>
       </c>
-      <c r="D20" s="14" t="s">
-        <v>54</v>
-      </c>
-      <c r="E20" s="14" t="s">
-        <v>55</v>
-      </c>
-      <c r="F20" s="17">
+      <c r="C23" s="13" t="s">
+        <v>19</v>
+      </c>
+      <c r="D23" s="13" t="s">
+        <v>19</v>
+      </c>
+      <c r="E23" s="13"/>
+      <c r="F23" s="18">
+        <v>44521.0</v>
+      </c>
+      <c r="G23" s="18">
+        <v>44521.0</v>
+      </c>
+      <c r="H23" s="16">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="24" ht="19.5" customHeight="1">
+      <c r="B24" s="19" t="s">
+        <v>63</v>
+      </c>
+      <c r="C24" s="20"/>
+      <c r="D24" s="20"/>
+      <c r="E24" s="20"/>
+      <c r="F24" s="24">
         <v>44501.0</v>
       </c>
-      <c r="G20" s="17">
-        <v>44514.0</v>
-      </c>
-      <c r="H20" s="16">
-        <v>0.0</v>
-      </c>
-    </row>
-    <row r="21" ht="19.5" customHeight="1">
-      <c r="B21" s="22" t="s">
-        <v>56</v>
-      </c>
-      <c r="C21" s="14" t="s">
-        <v>57</v>
-      </c>
-      <c r="D21" s="14" t="s">
-        <v>58</v>
-      </c>
-      <c r="E21" s="14" t="s">
-        <v>59</v>
-      </c>
-      <c r="F21" s="17">
-        <v>44501.0</v>
-      </c>
-      <c r="G21" s="17">
+      <c r="G24" s="24">
         <v>44521.0</v>
       </c>
-      <c r="H21" s="16">
-        <v>0.0</v>
-      </c>
-    </row>
-    <row r="22" ht="19.5" customHeight="1">
-      <c r="B22" s="13" t="s">
-        <v>50</v>
-      </c>
-      <c r="C22" s="13" t="s">
-        <v>19</v>
-      </c>
-      <c r="D22" s="13" t="s">
-        <v>19</v>
-      </c>
-      <c r="E22" s="13"/>
-      <c r="F22" s="17">
-        <v>44521.0</v>
-      </c>
-      <c r="G22" s="17">
-        <v>44521.0</v>
-      </c>
-      <c r="H22" s="16">
-        <v>0.0</v>
-      </c>
-    </row>
-    <row r="23" ht="19.5" customHeight="1">
-      <c r="B23" s="18" t="s">
-        <v>60</v>
-      </c>
-      <c r="C23" s="19"/>
-      <c r="D23" s="19"/>
-      <c r="E23" s="19"/>
-      <c r="F23" s="23">
-        <v>44501.0</v>
-      </c>
-      <c r="G23" s="23">
-        <v>44521.0</v>
-      </c>
-      <c r="H23" s="21">
-        <f>(H20+H21+H22)/3</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="24" ht="19.5" customHeight="1">
-      <c r="B24" s="14" t="s">
-        <v>61</v>
-      </c>
-      <c r="C24" s="14" t="s">
-        <v>62</v>
-      </c>
-      <c r="D24" s="14" t="s">
-        <v>63</v>
-      </c>
-      <c r="E24" s="14" t="s">
+      <c r="H24" s="22">
+        <f>(H21+H22+H23)/3</f>
+        <v>0.4333333333</v>
+      </c>
+    </row>
+    <row r="25" ht="19.5" customHeight="1">
+      <c r="B25" s="14" t="s">
         <v>64</v>
       </c>
-      <c r="F24" s="17">
+      <c r="C25" s="14" t="s">
+        <v>65</v>
+      </c>
+      <c r="D25" s="14" t="s">
+        <v>66</v>
+      </c>
+      <c r="E25" s="14" t="s">
+        <v>67</v>
+      </c>
+      <c r="F25" s="18">
         <v>44522.0</v>
       </c>
-      <c r="G24" s="17">
-        <v>44542.0</v>
-      </c>
-      <c r="H24" s="16">
-        <v>0.0</v>
-      </c>
-    </row>
-    <row r="25" ht="19.5" customHeight="1">
-      <c r="B25" s="13" t="s">
-        <v>65</v>
-      </c>
-      <c r="C25" s="13" t="s">
-        <v>66</v>
-      </c>
-      <c r="D25" s="14" t="s">
-        <v>67</v>
-      </c>
-      <c r="E25" s="14" t="s">
-        <v>68</v>
-      </c>
-      <c r="F25" s="17">
-        <v>44522.0</v>
-      </c>
-      <c r="G25" s="17">
+      <c r="G25" s="18">
         <v>44542.0</v>
       </c>
       <c r="H25" s="16">
@@ -1198,26 +1215,23 @@
       </c>
     </row>
     <row r="26" ht="19.5" customHeight="1">
-      <c r="A26" s="2" t="s">
-        <v>29</v>
-      </c>
       <c r="B26" s="13" t="s">
+        <v>68</v>
+      </c>
+      <c r="C26" s="13" t="s">
         <v>69</v>
       </c>
-      <c r="C26" s="13" t="s">
+      <c r="D26" s="14" t="s">
         <v>70</v>
       </c>
-      <c r="D26" s="14" t="s">
+      <c r="E26" s="14" t="s">
         <v>71</v>
       </c>
-      <c r="E26" s="14" t="s">
-        <v>72</v>
-      </c>
-      <c r="F26" s="17">
+      <c r="F26" s="18">
+        <v>44522.0</v>
+      </c>
+      <c r="G26" s="18">
         <v>44542.0</v>
-      </c>
-      <c r="G26" s="17">
-        <v>44549.0</v>
       </c>
       <c r="H26" s="16">
         <v>0.0</v>
@@ -1225,24 +1239,24 @@
     </row>
     <row r="27" ht="19.5" customHeight="1">
       <c r="A27" s="2" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="B27" s="13" t="s">
+        <v>72</v>
+      </c>
+      <c r="C27" s="13" t="s">
         <v>73</v>
       </c>
-      <c r="C27" s="13" t="s">
+      <c r="D27" s="14" t="s">
         <v>74</v>
       </c>
-      <c r="D27" s="14" t="s">
+      <c r="E27" s="14" t="s">
         <v>75</v>
       </c>
-      <c r="E27" s="14" t="s">
-        <v>76</v>
-      </c>
-      <c r="F27" s="17">
+      <c r="F27" s="18">
         <v>44542.0</v>
       </c>
-      <c r="G27" s="17">
+      <c r="G27" s="18">
         <v>44549.0</v>
       </c>
       <c r="H27" s="16">
@@ -1250,20 +1264,25 @@
       </c>
     </row>
     <row r="28" ht="19.5" customHeight="1">
+      <c r="A28" s="2" t="s">
+        <v>32</v>
+      </c>
       <c r="B28" s="13" t="s">
-        <v>50</v>
+        <v>76</v>
       </c>
       <c r="C28" s="13" t="s">
-        <v>19</v>
-      </c>
-      <c r="D28" s="13" t="s">
-        <v>19</v>
-      </c>
-      <c r="E28" s="13"/>
-      <c r="F28" s="17">
-        <v>44549.0</v>
-      </c>
-      <c r="G28" s="17">
+        <v>77</v>
+      </c>
+      <c r="D28" s="14" t="s">
+        <v>78</v>
+      </c>
+      <c r="E28" s="14" t="s">
+        <v>79</v>
+      </c>
+      <c r="F28" s="18">
+        <v>44542.0</v>
+      </c>
+      <c r="G28" s="18">
         <v>44549.0</v>
       </c>
       <c r="H28" s="16">
@@ -1271,24 +1290,44 @@
       </c>
     </row>
     <row r="29" ht="19.5" customHeight="1">
-      <c r="B29" s="18" t="s">
-        <v>77</v>
-      </c>
-      <c r="C29" s="19"/>
-      <c r="D29" s="19"/>
-      <c r="E29" s="19"/>
-      <c r="F29" s="24">
+      <c r="B29" s="13" t="s">
+        <v>53</v>
+      </c>
+      <c r="C29" s="13" t="s">
+        <v>19</v>
+      </c>
+      <c r="D29" s="13" t="s">
+        <v>19</v>
+      </c>
+      <c r="E29" s="13"/>
+      <c r="F29" s="18">
+        <v>44549.0</v>
+      </c>
+      <c r="G29" s="18">
+        <v>44549.0</v>
+      </c>
+      <c r="H29" s="16">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="30" ht="19.5" customHeight="1">
+      <c r="B30" s="19" t="s">
+        <v>80</v>
+      </c>
+      <c r="C30" s="20"/>
+      <c r="D30" s="20"/>
+      <c r="E30" s="20"/>
+      <c r="F30" s="25">
         <v>44522.0</v>
       </c>
-      <c r="G29" s="23">
+      <c r="G30" s="24">
         <v>44549.0</v>
       </c>
-      <c r="H29" s="21">
-        <f>(H24+ H25+H26+H27+H28)/5</f>
+      <c r="H30" s="22">
+        <f>(H25+ H26+H27+H28+H29)/5</f>
         <v>0</v>
       </c>
     </row>
-    <row r="30" ht="15.75" customHeight="1"/>
     <row r="31" ht="15.75" customHeight="1"/>
     <row r="32" ht="15.75" customHeight="1"/>
     <row r="33" ht="15.75" customHeight="1"/>
@@ -2233,6 +2272,7 @@
     <row r="972" ht="15.75" customHeight="1"/>
     <row r="973" ht="15.75" customHeight="1"/>
     <row r="974" ht="15.75" customHeight="1"/>
+    <row r="975" ht="15.75" customHeight="1"/>
   </sheetData>
   <mergeCells count="2">
     <mergeCell ref="B1:H1"/>
@@ -2266,106 +2306,106 @@
   <sheetData>
     <row r="2" ht="15.0" customHeight="1">
       <c r="B2" s="2" t="s">
-        <v>78</v>
+        <v>81</v>
       </c>
     </row>
     <row r="4" ht="18.0" customHeight="1">
-      <c r="B4" s="25" t="s">
-        <v>79</v>
-      </c>
-      <c r="C4" s="25" t="s">
-        <v>80</v>
-      </c>
-      <c r="D4" s="25" t="s">
-        <v>81</v>
+      <c r="B4" s="26" t="s">
+        <v>82</v>
+      </c>
+      <c r="C4" s="26" t="s">
+        <v>83</v>
+      </c>
+      <c r="D4" s="26" t="s">
+        <v>84</v>
       </c>
     </row>
     <row r="5" ht="15.0" customHeight="1">
-      <c r="B5" s="26" t="s">
-        <v>82</v>
+      <c r="B5" s="27" t="s">
+        <v>85</v>
       </c>
       <c r="C5" s="13" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="D5" s="14" t="s">
-        <v>84</v>
+        <v>87</v>
       </c>
     </row>
     <row r="6" ht="15.0" customHeight="1">
-      <c r="B6" s="27" t="s">
-        <v>85</v>
+      <c r="B6" s="28" t="s">
+        <v>88</v>
       </c>
       <c r="C6" s="13" t="s">
-        <v>86</v>
+        <v>89</v>
       </c>
       <c r="D6" s="13" t="s">
-        <v>87</v>
+        <v>90</v>
       </c>
     </row>
     <row r="7" ht="15.0" customHeight="1">
-      <c r="B7" s="27" t="s">
-        <v>88</v>
+      <c r="B7" s="28" t="s">
+        <v>91</v>
       </c>
       <c r="C7" s="13" t="s">
+        <v>92</v>
+      </c>
+      <c r="D7" s="13" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="8" ht="15.0" customHeight="1">
+      <c r="B8" s="28" t="s">
+        <v>94</v>
+      </c>
+      <c r="C8" s="14" t="s">
         <v>89</v>
       </c>
-      <c r="D7" s="13" t="s">
+      <c r="D8" s="14" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="8" ht="15.0" customHeight="1">
-      <c r="B8" s="27" t="s">
-        <v>91</v>
-      </c>
-      <c r="C8" s="14" t="s">
-        <v>86</v>
-      </c>
-      <c r="D8" s="14" t="s">
-        <v>87</v>
-      </c>
-    </row>
     <row r="9" ht="15.0" customHeight="1">
-      <c r="B9" s="27" t="s">
+      <c r="B9" s="28" t="s">
+        <v>95</v>
+      </c>
+      <c r="C9" s="13" t="s">
         <v>92</v>
       </c>
-      <c r="C9" s="13" t="s">
-        <v>89</v>
-      </c>
       <c r="D9" s="13" t="s">
-        <v>90</v>
+        <v>93</v>
       </c>
     </row>
     <row r="10" ht="15.0" customHeight="1">
-      <c r="B10" s="28" t="s">
-        <v>93</v>
-      </c>
-      <c r="C10" s="29" t="s">
-        <v>94</v>
-      </c>
-      <c r="D10" s="29" t="s">
-        <v>95</v>
+      <c r="B10" s="29" t="s">
+        <v>96</v>
+      </c>
+      <c r="C10" s="30" t="s">
+        <v>97</v>
+      </c>
+      <c r="D10" s="30" t="s">
+        <v>98</v>
       </c>
     </row>
     <row r="11">
-      <c r="B11" s="30" t="s">
-        <v>96</v>
-      </c>
-      <c r="C11" s="30" t="s">
-        <v>97</v>
-      </c>
-      <c r="D11" s="30" t="s">
-        <v>98</v>
+      <c r="B11" s="31" t="s">
+        <v>99</v>
+      </c>
+      <c r="C11" s="31" t="s">
+        <v>100</v>
+      </c>
+      <c r="D11" s="31" t="s">
+        <v>101</v>
       </c>
     </row>
     <row r="12">
-      <c r="B12" s="22" t="s">
-        <v>99</v>
-      </c>
-      <c r="C12" s="22" t="s">
-        <v>100</v>
-      </c>
-      <c r="D12" s="22" t="s">
-        <v>101</v>
+      <c r="B12" s="23" t="s">
+        <v>102</v>
+      </c>
+      <c r="C12" s="23" t="s">
+        <v>103</v>
+      </c>
+      <c r="D12" s="23" t="s">
+        <v>104</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
SE SUBE SEGUN CRONOGRAMA EL MODULO PROFESOR A LA LINEA BASE 02(FALTAN ALGUNAS FUNCIONALIDADES QUE NECESITAN DEL MODULO ALUMNO PARA FUNCIONAR CORRECTAMENTE)
</commit_message>
<xml_diff>
--- a/Desarrollo/SACNS/gestion/SACNS-DCP.xlsx
+++ b/Desarrollo/SACNS/gestion/SACNS-DCP.xlsx
@@ -1,13 +1,33 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24527"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\xampp\GCS-G5\Desarrollo\SACNS\gestion\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E22AA2A6-BD6C-48CC-8AB7-7099E988A996}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <bookViews>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+  </bookViews>
   <sheets>
-    <sheet state="visible" name="Cronograma" sheetId="1" r:id="rId4"/>
-    <sheet state="visible" name="Miembros del Grupo" sheetId="2" r:id="rId5"/>
+    <sheet name="Cronograma" sheetId="1" r:id="rId1"/>
+    <sheet name="Miembros del Grupo" sheetId="2" r:id="rId2"/>
   </sheets>
-  <definedNames/>
-  <calcPr/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -332,7 +352,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="3">
     <numFmt numFmtId="164" formatCode="d/m/yyyy"/>
     <numFmt numFmtId="165" formatCode="dd&quot;/&quot;mm&quot;/&quot;yyyy"/>
@@ -340,48 +360,49 @@
   </numFmts>
   <fonts count="9">
     <font>
-      <sz val="11.0"/>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Arial"/>
     </font>
     <font>
       <b/>
-      <sz val="11.0"/>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
     </font>
     <font>
-      <sz val="11.0"/>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
     </font>
     <font>
       <u/>
-      <sz val="11.0"/>
+      <sz val="11"/>
       <color rgb="FF1155CC"/>
       <name val="Arial"/>
     </font>
     <font>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
     </font>
     <font>
-      <sz val="11.0"/>
+      <sz val="11"/>
       <name val="Calibri"/>
     </font>
     <font>
-      <sz val="11.0"/>
+      <sz val="11"/>
       <color rgb="FFFF0000"/>
       <name val="Calibri"/>
     </font>
     <font>
       <b/>
-      <sz val="13.0"/>
+      <sz val="13"/>
       <color theme="1"/>
       <name val="Calibri"/>
     </font>
     <font>
-      <sz val="11.0"/>
+      <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
     </font>
@@ -391,7 +412,7 @@
       <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="lightGray"/>
+      <patternFill patternType="gray125"/>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -425,7 +446,13 @@
     </fill>
   </fills>
   <borders count="3">
-    <border/>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
     <border>
       <left style="thin">
         <color rgb="FF000000"/>
@@ -439,6 +466,7 @@
       <bottom style="thin">
         <color rgb="FF000000"/>
       </bottom>
+      <diagonal/>
     </border>
     <border>
       <left style="thin">
@@ -450,112 +478,82 @@
       <top style="thin">
         <color rgb="FF000000"/>
       </top>
+      <bottom/>
+      <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="32">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
+  <cellXfs count="33">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
-    <xf borderId="0" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="165" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="9" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="166" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="9" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="166" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="164" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="right" readingOrder="0"/>
-    </xf>
-    <xf borderId="1" fillId="3" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFill="1" applyFont="1"/>
-    <xf borderId="1" fillId="4" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
-      <alignment horizontal="right" readingOrder="0"/>
-    </xf>
-    <xf borderId="1" fillId="4" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
-    </xf>
-    <xf borderId="1" fillId="4" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0" vertical="center"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="1" fillId="4" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf borderId="1" fillId="4" fontId="2" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="right" readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf borderId="1" fillId="2" fontId="1" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="1" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="1" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="1" fillId="0" fontId="2" numFmtId="165" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="1" fillId="0" fontId="2" numFmtId="9" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="1" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="1" fillId="0" fontId="2" numFmtId="166" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="1" fillId="2" fontId="6" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="1" fillId="2" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="1" fillId="2" fontId="2" numFmtId="165" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="1" fillId="2" fontId="2" numFmtId="9" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="1" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="1" fillId="2" fontId="2" numFmtId="166" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="1" fillId="2" fontId="2" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="1" fillId="5" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf borderId="1" fillId="6" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="1" fillId="0" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="2" fillId="0" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="2" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="2" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle xfId="0" name="Normal" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
-<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheets">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Sheets">
   <a:themeElements>
     <a:clrScheme name="Sheets">
       <a:dk1>
@@ -745,591 +743,596 @@
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-  <sheetPr>
-    <pageSetUpPr/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:H975"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I23" sqref="I23"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="12.59765625" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="4.88"/>
-    <col customWidth="1" min="2" max="2" width="32.88"/>
-    <col customWidth="1" min="3" max="3" width="33.0"/>
-    <col customWidth="1" min="4" max="4" width="21.38"/>
-    <col customWidth="1" min="5" max="5" width="52.5"/>
-    <col customWidth="1" min="6" max="7" width="9.88"/>
-    <col customWidth="1" min="8" max="8" width="10.5"/>
-    <col customWidth="1" min="9" max="26" width="9.38"/>
+    <col min="1" max="1" width="4.8984375" customWidth="1"/>
+    <col min="2" max="2" width="32.8984375" customWidth="1"/>
+    <col min="3" max="3" width="33" customWidth="1"/>
+    <col min="4" max="4" width="21.3984375" customWidth="1"/>
+    <col min="5" max="5" width="52.5" customWidth="1"/>
+    <col min="6" max="7" width="9.8984375" customWidth="1"/>
+    <col min="8" max="8" width="10.5" customWidth="1"/>
+    <col min="9" max="26" width="9.3984375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1">
-      <c r="B1" s="1" t="s">
+    <row r="1" spans="1:8" ht="14.4">
+      <c r="B1" s="30" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="2">
-      <c r="B2" s="2" t="s">
+      <c r="C1" s="31"/>
+      <c r="D1" s="31"/>
+      <c r="E1" s="31"/>
+      <c r="F1" s="31"/>
+      <c r="G1" s="31"/>
+      <c r="H1" s="31"/>
+    </row>
+    <row r="2" spans="1:8" ht="14.4">
+      <c r="B2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C2" s="32" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="3">
-      <c r="B3" s="4" t="s">
+      <c r="D2" s="31"/>
+    </row>
+    <row r="3" spans="1:8" ht="14.4">
+      <c r="B3" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="C3" s="5">
-        <v>5.0</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="B4" s="4" t="s">
+      <c r="C3" s="3">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" ht="28.8">
+      <c r="B4" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C4" s="6" t="s">
+      <c r="C4" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="D4" s="7" t="s">
+      <c r="D4" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="E4" s="8"/>
-    </row>
-    <row r="5">
-      <c r="B5" s="4" t="s">
+      <c r="E4" s="6"/>
+    </row>
+    <row r="5" spans="1:8" ht="14.4">
+      <c r="B5" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C5" s="9" t="s">
+      <c r="C5" s="7" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="6">
-      <c r="B6" s="4" t="s">
+    <row r="6" spans="1:8" ht="14.4">
+      <c r="B6" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="C6" s="10">
-        <v>44480.0</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="B7" s="4" t="s">
+      <c r="C6" s="8">
+        <v>44480</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" ht="14.4">
+      <c r="B7" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="C7" s="10">
-        <v>44550.0</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="B8" s="11"/>
-      <c r="C8" s="11"/>
-      <c r="E8" s="11"/>
-      <c r="F8" s="11"/>
-      <c r="G8" s="11"/>
-      <c r="H8" s="11"/>
-    </row>
-    <row r="9">
-      <c r="B9" s="12" t="s">
+      <c r="C7" s="8">
+        <v>44550</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" ht="14.4">
+      <c r="B8" s="9"/>
+      <c r="C8" s="9"/>
+      <c r="E8" s="9"/>
+      <c r="F8" s="9"/>
+      <c r="G8" s="9"/>
+      <c r="H8" s="9"/>
+    </row>
+    <row r="9" spans="1:8" ht="14.4">
+      <c r="B9" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="C9" s="12" t="s">
+      <c r="C9" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="D9" s="12" t="s">
+      <c r="D9" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="E9" s="12" t="s">
+      <c r="E9" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="F9" s="12" t="s">
+      <c r="F9" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="G9" s="12" t="s">
+      <c r="G9" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="H9" s="12" t="s">
+      <c r="H9" s="10" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="10" ht="19.5" customHeight="1">
-      <c r="B10" s="13" t="s">
+    <row r="10" spans="1:8" ht="19.5" customHeight="1">
+      <c r="B10" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="C10" s="13" t="s">
+      <c r="C10" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="D10" s="13" t="s">
+      <c r="D10" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="E10" s="14" t="s">
+      <c r="E10" s="12" t="s">
         <v>20</v>
       </c>
-      <c r="F10" s="15">
-        <v>44480.0</v>
-      </c>
-      <c r="G10" s="15">
-        <v>44487.0</v>
-      </c>
-      <c r="H10" s="16">
-        <v>1.0</v>
-      </c>
-    </row>
-    <row r="11" ht="19.5" customHeight="1">
-      <c r="B11" s="14" t="s">
+      <c r="F10" s="13">
+        <v>44480</v>
+      </c>
+      <c r="G10" s="13">
+        <v>44487</v>
+      </c>
+      <c r="H10" s="14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" ht="19.5" customHeight="1">
+      <c r="B11" s="12" t="s">
         <v>21</v>
       </c>
-      <c r="C11" s="14" t="s">
+      <c r="C11" s="12" t="s">
         <v>22</v>
       </c>
-      <c r="D11" s="14" t="s">
+      <c r="D11" s="12" t="s">
         <v>23</v>
       </c>
-      <c r="E11" s="14" t="s">
+      <c r="E11" s="12" t="s">
         <v>24</v>
       </c>
-      <c r="F11" s="15">
-        <v>44480.0</v>
-      </c>
-      <c r="G11" s="15">
-        <v>44487.0</v>
-      </c>
-      <c r="H11" s="16">
-        <v>1.0</v>
-      </c>
-    </row>
-    <row r="12" ht="19.5" customHeight="1">
-      <c r="B12" s="13" t="s">
+      <c r="F11" s="13">
+        <v>44480</v>
+      </c>
+      <c r="G11" s="13">
+        <v>44487</v>
+      </c>
+      <c r="H11" s="14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" ht="19.5" customHeight="1">
+      <c r="B12" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="C12" s="13" t="s">
+      <c r="C12" s="11" t="s">
         <v>26</v>
       </c>
-      <c r="D12" s="14" t="s">
+      <c r="D12" s="12" t="s">
         <v>27</v>
       </c>
-      <c r="E12" s="14" t="s">
+      <c r="E12" s="12" t="s">
         <v>28</v>
       </c>
-      <c r="F12" s="15">
-        <v>44480.0</v>
-      </c>
-      <c r="G12" s="15">
-        <v>44487.0</v>
-      </c>
-      <c r="H12" s="16">
-        <v>1.0</v>
-      </c>
-    </row>
-    <row r="13" ht="19.5" customHeight="1">
-      <c r="A13" s="2"/>
-      <c r="B13" s="17" t="s">
+      <c r="F12" s="13">
+        <v>44480</v>
+      </c>
+      <c r="G12" s="13">
+        <v>44487</v>
+      </c>
+      <c r="H12" s="14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" ht="19.5" customHeight="1">
+      <c r="A13" s="1"/>
+      <c r="B13" s="15" t="s">
         <v>29</v>
       </c>
-      <c r="C13" s="17" t="s">
+      <c r="C13" s="15" t="s">
         <v>30</v>
       </c>
-      <c r="D13" s="14" t="s">
+      <c r="D13" s="12" t="s">
         <v>31</v>
       </c>
-      <c r="E13" s="14" t="s">
+      <c r="E13" s="12" t="s">
         <v>24</v>
       </c>
-      <c r="F13" s="15">
-        <v>44480.0</v>
-      </c>
-      <c r="G13" s="15">
-        <v>44487.0</v>
-      </c>
-      <c r="H13" s="16">
-        <v>1.0</v>
-      </c>
-    </row>
-    <row r="14" ht="19.5" customHeight="1">
-      <c r="A14" s="2" t="s">
+      <c r="F13" s="13">
+        <v>44480</v>
+      </c>
+      <c r="G13" s="13">
+        <v>44487</v>
+      </c>
+      <c r="H13" s="14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" ht="19.5" customHeight="1">
+      <c r="A14" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="B14" s="13" t="s">
+      <c r="B14" s="11" t="s">
         <v>33</v>
       </c>
-      <c r="C14" s="13" t="s">
+      <c r="C14" s="11" t="s">
         <v>34</v>
       </c>
-      <c r="D14" s="14" t="s">
+      <c r="D14" s="12" t="s">
         <v>35</v>
       </c>
-      <c r="E14" s="14" t="s">
+      <c r="E14" s="12" t="s">
         <v>36</v>
       </c>
-      <c r="F14" s="15">
-        <v>44487.0</v>
-      </c>
-      <c r="G14" s="15">
-        <v>44494.0</v>
-      </c>
-      <c r="H14" s="16">
-        <v>1.0</v>
-      </c>
-    </row>
-    <row r="15" ht="19.5" customHeight="1">
-      <c r="B15" s="13" t="s">
+      <c r="F14" s="13">
+        <v>44487</v>
+      </c>
+      <c r="G14" s="13">
+        <v>44494</v>
+      </c>
+      <c r="H14" s="14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" ht="19.5" customHeight="1">
+      <c r="B15" s="11" t="s">
         <v>37</v>
       </c>
-      <c r="C15" s="13" t="s">
+      <c r="C15" s="11" t="s">
         <v>38</v>
       </c>
-      <c r="D15" s="14" t="s">
+      <c r="D15" s="12" t="s">
         <v>39</v>
       </c>
-      <c r="E15" s="14" t="s">
+      <c r="E15" s="12" t="s">
         <v>40</v>
       </c>
-      <c r="F15" s="15">
-        <v>44487.0</v>
-      </c>
-      <c r="G15" s="15">
-        <v>44494.0</v>
-      </c>
-      <c r="H15" s="16">
-        <v>1.0</v>
-      </c>
-    </row>
-    <row r="16" ht="19.5" customHeight="1">
-      <c r="B16" s="13" t="s">
+      <c r="F15" s="13">
+        <v>44487</v>
+      </c>
+      <c r="G15" s="13">
+        <v>44494</v>
+      </c>
+      <c r="H15" s="14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" ht="19.5" customHeight="1">
+      <c r="B16" s="11" t="s">
         <v>41</v>
       </c>
-      <c r="C16" s="13" t="s">
+      <c r="C16" s="11" t="s">
         <v>42</v>
       </c>
-      <c r="D16" s="14" t="s">
+      <c r="D16" s="12" t="s">
         <v>43</v>
       </c>
-      <c r="E16" s="14" t="s">
+      <c r="E16" s="12" t="s">
         <v>44</v>
       </c>
-      <c r="F16" s="15">
-        <v>44487.0</v>
-      </c>
-      <c r="G16" s="15">
-        <v>44494.0</v>
-      </c>
-      <c r="H16" s="16">
-        <v>1.0</v>
-      </c>
-    </row>
-    <row r="17" ht="19.5" customHeight="1">
-      <c r="B17" s="13" t="s">
+      <c r="F16" s="13">
+        <v>44487</v>
+      </c>
+      <c r="G16" s="13">
+        <v>44494</v>
+      </c>
+      <c r="H16" s="14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" ht="19.5" customHeight="1">
+      <c r="B17" s="11" t="s">
         <v>45</v>
       </c>
-      <c r="C17" s="13" t="s">
+      <c r="C17" s="11" t="s">
         <v>46</v>
       </c>
-      <c r="D17" s="14" t="s">
+      <c r="D17" s="12" t="s">
         <v>47</v>
       </c>
-      <c r="E17" s="14" t="s">
+      <c r="E17" s="12" t="s">
         <v>48</v>
       </c>
-      <c r="F17" s="15">
-        <v>44487.0</v>
-      </c>
-      <c r="G17" s="15">
-        <v>44494.0</v>
-      </c>
-      <c r="H17" s="16">
-        <v>1.0</v>
-      </c>
-    </row>
-    <row r="18" ht="19.5" customHeight="1">
-      <c r="B18" s="14" t="s">
+      <c r="F17" s="13">
+        <v>44487</v>
+      </c>
+      <c r="G17" s="13">
+        <v>44494</v>
+      </c>
+      <c r="H17" s="14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" ht="19.5" customHeight="1">
+      <c r="B18" s="12" t="s">
         <v>49</v>
       </c>
-      <c r="C18" s="13" t="s">
+      <c r="C18" s="11" t="s">
         <v>50</v>
       </c>
-      <c r="D18" s="14" t="s">
+      <c r="D18" s="12" t="s">
         <v>51</v>
       </c>
-      <c r="E18" s="14" t="s">
+      <c r="E18" s="12" t="s">
         <v>52</v>
       </c>
-      <c r="F18" s="15">
-        <v>44493.0</v>
-      </c>
-      <c r="G18" s="15">
-        <v>44500.0</v>
-      </c>
-      <c r="H18" s="16">
-        <v>1.0</v>
-      </c>
-    </row>
-    <row r="19" ht="19.5" customHeight="1">
-      <c r="B19" s="13" t="s">
+      <c r="F18" s="13">
+        <v>44493</v>
+      </c>
+      <c r="G18" s="13">
+        <v>44500</v>
+      </c>
+      <c r="H18" s="14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" ht="19.5" customHeight="1">
+      <c r="B19" s="11" t="s">
         <v>53</v>
       </c>
-      <c r="C19" s="13" t="s">
+      <c r="C19" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="D19" s="13" t="s">
+      <c r="D19" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="E19" s="13"/>
-      <c r="F19" s="15">
-        <v>44501.0</v>
-      </c>
-      <c r="G19" s="18">
-        <v>44501.0</v>
-      </c>
-      <c r="H19" s="16">
-        <v>1.0</v>
-      </c>
-    </row>
-    <row r="20" ht="19.5" customHeight="1">
-      <c r="B20" s="19" t="s">
+      <c r="E19" s="11"/>
+      <c r="F19" s="13">
+        <v>44501</v>
+      </c>
+      <c r="G19" s="16">
+        <v>44501</v>
+      </c>
+      <c r="H19" s="14"/>
+    </row>
+    <row r="20" spans="1:8" ht="19.5" customHeight="1">
+      <c r="B20" s="17" t="s">
         <v>54</v>
       </c>
-      <c r="C20" s="20"/>
-      <c r="D20" s="20"/>
-      <c r="E20" s="20"/>
-      <c r="F20" s="21">
-        <v>44480.0</v>
-      </c>
-      <c r="G20" s="21">
-        <v>44501.0</v>
-      </c>
-      <c r="H20" s="22">
-        <f>(H10+H11+H12+H14+H15+H16+H17+H18+H19)/9</f>
+      <c r="C20" s="18"/>
+      <c r="D20" s="18"/>
+      <c r="E20" s="18"/>
+      <c r="F20" s="19">
+        <v>44480</v>
+      </c>
+      <c r="G20" s="19">
+        <v>44501</v>
+      </c>
+      <c r="H20" s="20">
+        <f>(H10+H11+H12+H14+H15+H16+H17+H18)/8</f>
         <v>1</v>
       </c>
     </row>
-    <row r="21" ht="19.5" customHeight="1">
-      <c r="B21" s="13" t="s">
+    <row r="21" spans="1:8" ht="19.5" customHeight="1">
+      <c r="B21" s="11" t="s">
         <v>55</v>
       </c>
-      <c r="C21" s="13" t="s">
+      <c r="C21" s="11" t="s">
         <v>56</v>
       </c>
-      <c r="D21" s="14" t="s">
+      <c r="D21" s="12" t="s">
         <v>57</v>
       </c>
-      <c r="E21" s="14" t="s">
+      <c r="E21" s="12" t="s">
         <v>58</v>
       </c>
-      <c r="F21" s="18">
-        <v>44501.0</v>
-      </c>
-      <c r="G21" s="18">
-        <v>44514.0</v>
-      </c>
-      <c r="H21" s="16">
-        <v>1.0</v>
-      </c>
-    </row>
-    <row r="22" ht="19.5" customHeight="1">
-      <c r="B22" s="23" t="s">
+      <c r="F21" s="16">
+        <v>44501</v>
+      </c>
+      <c r="G21" s="16">
+        <v>44514</v>
+      </c>
+      <c r="H21" s="14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" ht="19.5" customHeight="1">
+      <c r="B22" s="21" t="s">
         <v>59</v>
       </c>
-      <c r="C22" s="14" t="s">
+      <c r="C22" s="12" t="s">
         <v>60</v>
       </c>
-      <c r="D22" s="14" t="s">
+      <c r="D22" s="12" t="s">
         <v>61</v>
       </c>
-      <c r="E22" s="14" t="s">
+      <c r="E22" s="12" t="s">
         <v>62</v>
       </c>
-      <c r="F22" s="18">
-        <v>44501.0</v>
-      </c>
-      <c r="G22" s="18">
-        <v>44521.0</v>
-      </c>
-      <c r="H22" s="16">
-        <v>0.3</v>
-      </c>
-    </row>
-    <row r="23" ht="19.5" customHeight="1">
-      <c r="B23" s="13" t="s">
+      <c r="F22" s="16">
+        <v>44501</v>
+      </c>
+      <c r="G22" s="16">
+        <v>44521</v>
+      </c>
+      <c r="H22" s="14">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" ht="19.5" customHeight="1">
+      <c r="B23" s="11" t="s">
         <v>53</v>
       </c>
-      <c r="C23" s="13" t="s">
+      <c r="C23" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="D23" s="13" t="s">
+      <c r="D23" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="E23" s="13"/>
-      <c r="F23" s="18">
-        <v>44521.0</v>
-      </c>
-      <c r="G23" s="18">
-        <v>44521.0</v>
-      </c>
-      <c r="H23" s="16">
-        <v>0.0</v>
-      </c>
-    </row>
-    <row r="24" ht="19.5" customHeight="1">
-      <c r="B24" s="19" t="s">
+      <c r="E23" s="11"/>
+      <c r="F23" s="16">
+        <v>44521</v>
+      </c>
+      <c r="G23" s="16">
+        <v>44521</v>
+      </c>
+      <c r="H23" s="14"/>
+    </row>
+    <row r="24" spans="1:8" ht="19.5" customHeight="1">
+      <c r="B24" s="17" t="s">
         <v>63</v>
       </c>
-      <c r="C24" s="20"/>
-      <c r="D24" s="20"/>
-      <c r="E24" s="20"/>
-      <c r="F24" s="24">
-        <v>44501.0</v>
-      </c>
-      <c r="G24" s="24">
-        <v>44521.0</v>
-      </c>
-      <c r="H24" s="22">
-        <f>(H21+H22+H23)/3</f>
-        <v>0.4333333333</v>
-      </c>
-    </row>
-    <row r="25" ht="19.5" customHeight="1">
-      <c r="B25" s="14" t="s">
+      <c r="C24" s="18"/>
+      <c r="D24" s="18"/>
+      <c r="E24" s="18"/>
+      <c r="F24" s="22">
+        <v>44501</v>
+      </c>
+      <c r="G24" s="22">
+        <v>44521</v>
+      </c>
+      <c r="H24" s="20">
+        <f>(H21+H22)/2</f>
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" ht="19.5" customHeight="1">
+      <c r="B25" s="12" t="s">
         <v>64</v>
       </c>
-      <c r="C25" s="14" t="s">
+      <c r="C25" s="12" t="s">
         <v>65</v>
       </c>
-      <c r="D25" s="14" t="s">
+      <c r="D25" s="12" t="s">
         <v>66</v>
       </c>
-      <c r="E25" s="14" t="s">
+      <c r="E25" s="12" t="s">
         <v>67</v>
       </c>
-      <c r="F25" s="18">
-        <v>44522.0</v>
-      </c>
-      <c r="G25" s="18">
-        <v>44542.0</v>
-      </c>
-      <c r="H25" s="16">
-        <v>0.0</v>
-      </c>
-    </row>
-    <row r="26" ht="19.5" customHeight="1">
-      <c r="B26" s="13" t="s">
+      <c r="F25" s="16">
+        <v>44522</v>
+      </c>
+      <c r="G25" s="16">
+        <v>44542</v>
+      </c>
+      <c r="H25" s="14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" ht="19.5" customHeight="1">
+      <c r="B26" s="11" t="s">
         <v>68</v>
       </c>
-      <c r="C26" s="13" t="s">
+      <c r="C26" s="11" t="s">
         <v>69</v>
       </c>
-      <c r="D26" s="14" t="s">
+      <c r="D26" s="12" t="s">
         <v>70</v>
       </c>
-      <c r="E26" s="14" t="s">
+      <c r="E26" s="12" t="s">
         <v>71</v>
       </c>
-      <c r="F26" s="18">
-        <v>44522.0</v>
-      </c>
-      <c r="G26" s="18">
-        <v>44542.0</v>
-      </c>
-      <c r="H26" s="16">
-        <v>0.0</v>
-      </c>
-    </row>
-    <row r="27" ht="19.5" customHeight="1">
-      <c r="A27" s="2" t="s">
+      <c r="F26" s="16">
+        <v>44522</v>
+      </c>
+      <c r="G26" s="16">
+        <v>44542</v>
+      </c>
+      <c r="H26" s="14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" ht="19.5" customHeight="1">
+      <c r="A27" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="B27" s="13" t="s">
+      <c r="B27" s="11" t="s">
         <v>72</v>
       </c>
-      <c r="C27" s="13" t="s">
+      <c r="C27" s="11" t="s">
         <v>73</v>
       </c>
-      <c r="D27" s="14" t="s">
+      <c r="D27" s="12" t="s">
         <v>74</v>
       </c>
-      <c r="E27" s="14" t="s">
+      <c r="E27" s="12" t="s">
         <v>75</v>
       </c>
-      <c r="F27" s="18">
-        <v>44542.0</v>
-      </c>
-      <c r="G27" s="18">
-        <v>44549.0</v>
-      </c>
-      <c r="H27" s="16">
-        <v>0.0</v>
-      </c>
-    </row>
-    <row r="28" ht="19.5" customHeight="1">
-      <c r="A28" s="2" t="s">
+      <c r="F27" s="16">
+        <v>44542</v>
+      </c>
+      <c r="G27" s="16">
+        <v>44549</v>
+      </c>
+      <c r="H27" s="14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" ht="19.5" customHeight="1">
+      <c r="A28" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="B28" s="13" t="s">
+      <c r="B28" s="11" t="s">
         <v>76</v>
       </c>
-      <c r="C28" s="13" t="s">
+      <c r="C28" s="11" t="s">
         <v>77</v>
       </c>
-      <c r="D28" s="14" t="s">
+      <c r="D28" s="12" t="s">
         <v>78</v>
       </c>
-      <c r="E28" s="14" t="s">
+      <c r="E28" s="12" t="s">
         <v>79</v>
       </c>
-      <c r="F28" s="18">
-        <v>44542.0</v>
-      </c>
-      <c r="G28" s="18">
-        <v>44549.0</v>
-      </c>
-      <c r="H28" s="16">
-        <v>0.0</v>
-      </c>
-    </row>
-    <row r="29" ht="19.5" customHeight="1">
-      <c r="B29" s="13" t="s">
+      <c r="F28" s="16">
+        <v>44542</v>
+      </c>
+      <c r="G28" s="16">
+        <v>44549</v>
+      </c>
+      <c r="H28" s="14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" ht="19.5" customHeight="1">
+      <c r="B29" s="11" t="s">
         <v>53</v>
       </c>
-      <c r="C29" s="13" t="s">
+      <c r="C29" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="D29" s="13" t="s">
+      <c r="D29" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="E29" s="13"/>
-      <c r="F29" s="18">
-        <v>44549.0</v>
-      </c>
-      <c r="G29" s="18">
-        <v>44549.0</v>
-      </c>
-      <c r="H29" s="16">
-        <v>0.0</v>
-      </c>
-    </row>
-    <row r="30" ht="19.5" customHeight="1">
-      <c r="B30" s="19" t="s">
+      <c r="E29" s="11"/>
+      <c r="F29" s="16">
+        <v>44549</v>
+      </c>
+      <c r="G29" s="16">
+        <v>44549</v>
+      </c>
+      <c r="H29" s="14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" ht="19.5" customHeight="1">
+      <c r="B30" s="17" t="s">
         <v>80</v>
       </c>
-      <c r="C30" s="20"/>
-      <c r="D30" s="20"/>
-      <c r="E30" s="20"/>
-      <c r="F30" s="25">
-        <v>44522.0</v>
-      </c>
-      <c r="G30" s="24">
-        <v>44549.0</v>
-      </c>
-      <c r="H30" s="22">
+      <c r="C30" s="18"/>
+      <c r="D30" s="18"/>
+      <c r="E30" s="18"/>
+      <c r="F30" s="23">
+        <v>44522</v>
+      </c>
+      <c r="G30" s="22">
+        <v>44549</v>
+      </c>
+      <c r="H30" s="20">
         <f>(H25+ H26+H27+H28+H29)/5</f>
         <v>0</v>
       </c>
     </row>
-    <row r="31" ht="15.75" customHeight="1"/>
-    <row r="32" ht="15.75" customHeight="1"/>
+    <row r="31" spans="1:8" ht="15.75" customHeight="1"/>
+    <row r="32" spans="1:8" ht="15.75" customHeight="1"/>
     <row r="33" ht="15.75" customHeight="1"/>
     <row r="34" ht="15.75" customHeight="1"/>
     <row r="35" ht="15.75" customHeight="1"/>
@@ -2279,139 +2282,135 @@
     <mergeCell ref="C2:D2"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink r:id="rId1" ref="C2"/>
+    <hyperlink ref="C2" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
   </hyperlinks>
-  <printOptions/>
-  <pageMargins bottom="0.75" footer="0.0" header="0.0" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup paperSize="9" orientation="portrait"/>
-  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
-    <pageSetUpPr/>
   </sheetPr>
+  <dimension ref="B2:D12"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="12.59765625" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col customWidth="1" min="2" max="2" width="22.13"/>
-    <col customWidth="1" min="3" max="3" width="23.75"/>
-    <col customWidth="1" min="4" max="4" width="15.75"/>
+    <col min="2" max="2" width="22.09765625" customWidth="1"/>
+    <col min="3" max="3" width="23.69921875" customWidth="1"/>
+    <col min="4" max="4" width="15.69921875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" ht="15.0" customHeight="1">
-      <c r="B2" s="2" t="s">
+    <row r="2" spans="2:4" ht="15" customHeight="1">
+      <c r="B2" s="1" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="4" ht="18.0" customHeight="1">
-      <c r="B4" s="26" t="s">
+    <row r="4" spans="2:4" ht="18" customHeight="1">
+      <c r="B4" s="24" t="s">
         <v>82</v>
       </c>
-      <c r="C4" s="26" t="s">
+      <c r="C4" s="24" t="s">
         <v>83</v>
       </c>
-      <c r="D4" s="26" t="s">
+      <c r="D4" s="24" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="5" ht="15.0" customHeight="1">
-      <c r="B5" s="27" t="s">
+    <row r="5" spans="2:4" ht="15" customHeight="1">
+      <c r="B5" s="25" t="s">
         <v>85</v>
       </c>
-      <c r="C5" s="13" t="s">
+      <c r="C5" s="11" t="s">
         <v>86</v>
       </c>
-      <c r="D5" s="14" t="s">
+      <c r="D5" s="12" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="6" ht="15.0" customHeight="1">
-      <c r="B6" s="28" t="s">
+    <row r="6" spans="2:4" ht="15" customHeight="1">
+      <c r="B6" s="26" t="s">
         <v>88</v>
       </c>
-      <c r="C6" s="13" t="s">
+      <c r="C6" s="11" t="s">
         <v>89</v>
       </c>
-      <c r="D6" s="13" t="s">
+      <c r="D6" s="11" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="7" ht="15.0" customHeight="1">
-      <c r="B7" s="28" t="s">
+    <row r="7" spans="2:4" ht="15" customHeight="1">
+      <c r="B7" s="26" t="s">
         <v>91</v>
       </c>
-      <c r="C7" s="13" t="s">
+      <c r="C7" s="11" t="s">
         <v>92</v>
       </c>
-      <c r="D7" s="13" t="s">
+      <c r="D7" s="11" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="8" ht="15.0" customHeight="1">
-      <c r="B8" s="28" t="s">
+    <row r="8" spans="2:4" ht="15" customHeight="1">
+      <c r="B8" s="26" t="s">
         <v>94</v>
       </c>
-      <c r="C8" s="14" t="s">
+      <c r="C8" s="12" t="s">
         <v>89</v>
       </c>
-      <c r="D8" s="14" t="s">
+      <c r="D8" s="12" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="9" ht="15.0" customHeight="1">
-      <c r="B9" s="28" t="s">
+    <row r="9" spans="2:4" ht="15" customHeight="1">
+      <c r="B9" s="26" t="s">
         <v>95</v>
       </c>
-      <c r="C9" s="13" t="s">
+      <c r="C9" s="11" t="s">
         <v>92</v>
       </c>
-      <c r="D9" s="13" t="s">
+      <c r="D9" s="11" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="10" ht="15.0" customHeight="1">
-      <c r="B10" s="29" t="s">
+    <row r="10" spans="2:4" ht="15" customHeight="1">
+      <c r="B10" s="27" t="s">
         <v>96</v>
       </c>
-      <c r="C10" s="30" t="s">
+      <c r="C10" s="28" t="s">
         <v>97</v>
       </c>
-      <c r="D10" s="30" t="s">
+      <c r="D10" s="28" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="11">
-      <c r="B11" s="31" t="s">
+    <row r="11" spans="2:4" ht="14.4">
+      <c r="B11" s="29" t="s">
         <v>99</v>
       </c>
-      <c r="C11" s="31" t="s">
+      <c r="C11" s="29" t="s">
         <v>100</v>
       </c>
-      <c r="D11" s="31" t="s">
+      <c r="D11" s="29" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="12">
-      <c r="B12" s="23" t="s">
+    <row r="12" spans="2:4" ht="14.4">
+      <c r="B12" s="21" t="s">
         <v>102</v>
       </c>
-      <c r="C12" s="23" t="s">
+      <c r="C12" s="21" t="s">
         <v>103</v>
       </c>
-      <c r="D12" s="23" t="s">
+      <c r="D12" s="21" t="s">
         <v>104</v>
       </c>
     </row>
   </sheetData>
-  <printOptions/>
-  <pageMargins bottom="0.75" footer="0.0" header="0.0" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup orientation="landscape"/>
-  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
se actualiza porcentajes del avance del proyecto
</commit_message>
<xml_diff>
--- a/Desarrollo/SACNS/gestion/SACNS-DCP.xlsx
+++ b/Desarrollo/SACNS/gestion/SACNS-DCP.xlsx
@@ -1,33 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24527"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\xampp\GCS-G5\Desarrollo\SACNS\gestion\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E22AA2A6-BD6C-48CC-8AB7-7099E988A996}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
-  <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
-  </bookViews>
   <sheets>
-    <sheet name="Cronograma" sheetId="1" r:id="rId1"/>
-    <sheet name="Miembros del Grupo" sheetId="2" r:id="rId2"/>
+    <sheet state="visible" name="Cronograma" sheetId="1" r:id="rId4"/>
+    <sheet state="visible" name="Miembros del Grupo" sheetId="2" r:id="rId5"/>
   </sheets>
-  <calcPr calcId="191029"/>
-  <extLst>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
+  <definedNames/>
+  <calcPr/>
 </workbook>
 </file>
 
@@ -334,7 +314,7 @@
     <t>Balceda Delgado, Adriana</t>
   </si>
   <si>
-    <t>Admibistrador de BD</t>
+    <t>Administrador de BD</t>
   </si>
   <si>
     <t>BDA</t>
@@ -352,57 +332,52 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <numFmts count="3">
     <numFmt numFmtId="164" formatCode="d/m/yyyy"/>
     <numFmt numFmtId="165" formatCode="dd&quot;/&quot;mm&quot;/&quot;yyyy"/>
     <numFmt numFmtId="166" formatCode="dd/mm/yyyy"/>
   </numFmts>
-  <fonts count="9">
+  <fonts count="8">
     <font>
-      <sz val="11"/>
+      <sz val="11.0"/>
       <color theme="1"/>
       <name val="Arial"/>
     </font>
     <font>
       <b/>
-      <sz val="11"/>
+      <sz val="11.0"/>
       <color theme="1"/>
       <name val="Calibri"/>
     </font>
     <font>
-      <sz val="11"/>
+      <sz val="11.0"/>
       <color theme="1"/>
       <name val="Calibri"/>
     </font>
     <font>
       <u/>
-      <sz val="11"/>
+      <sz val="11.0"/>
       <color rgb="FF1155CC"/>
       <name val="Arial"/>
     </font>
     <font>
-      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
     </font>
     <font>
-      <sz val="11"/>
-      <name val="Calibri"/>
-    </font>
-    <font>
-      <sz val="11"/>
+      <sz val="11.0"/>
       <color rgb="FFFF0000"/>
       <name val="Calibri"/>
     </font>
     <font>
       <b/>
-      <sz val="13"/>
+      <sz val="13.0"/>
       <color theme="1"/>
       <name val="Calibri"/>
     </font>
     <font>
-      <sz val="11"/>
+      <sz val="11.0"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
     </font>
@@ -412,7 +387,7 @@
       <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="gray125"/>
+      <patternFill patternType="lightGray"/>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -446,13 +421,7 @@
     </fill>
   </fills>
   <borders count="3">
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
+    <border/>
     <border>
       <left style="thin">
         <color rgb="FF000000"/>
@@ -466,7 +435,6 @@
       <bottom style="thin">
         <color rgb="FF000000"/>
       </bottom>
-      <diagonal/>
     </border>
     <border>
       <left style="thin">
@@ -478,82 +446,109 @@
       <top style="thin">
         <color rgb="FF000000"/>
       </top>
-      <bottom/>
-      <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="33">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+  <cellXfs count="31">
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
+    </xf>
+    <xf borderId="0" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="right" readingOrder="0"/>
+    </xf>
+    <xf borderId="1" fillId="3" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFill="1" applyFont="1"/>
+    <xf borderId="1" fillId="4" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
+      <alignment horizontal="right" readingOrder="0"/>
+    </xf>
+    <xf borderId="1" fillId="4" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
+    </xf>
+    <xf borderId="1" fillId="4" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0" vertical="center"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="1" fillId="4" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf borderId="1" fillId="4" fontId="2" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment horizontal="right" readingOrder="0"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf borderId="1" fillId="2" fontId="1" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="1" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="1" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
+    <xf borderId="1" fillId="0" fontId="2" numFmtId="165" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment readingOrder="0"/>
     </xf>
-    <xf numFmtId="164" fontId="2" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
+    <xf borderId="1" fillId="0" fontId="2" numFmtId="9" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment readingOrder="0"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="165" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="9" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="166" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="9" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="166" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="164" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf borderId="1" fillId="0" fontId="2" numFmtId="166" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="1" fillId="2" fontId="5" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="1" fillId="2" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="1" fillId="2" fontId="2" numFmtId="165" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="1" fillId="2" fontId="2" numFmtId="9" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="1" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="1" fillId="2" fontId="2" numFmtId="166" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="1" fillId="2" fontId="2" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="1" fillId="5" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf borderId="1" fillId="6" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
+      <alignment readingOrder="0"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
+    <xf borderId="1" fillId="0" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="2" fillId="0" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="2" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="2" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle xfId="0" name="Normal" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Sheets">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheets">
   <a:themeElements>
     <a:clrScheme name="Sheets">
       <a:dk1>
@@ -743,596 +738,591 @@
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
-  <a:objectDefaults/>
-  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H975"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+  <sheetPr>
+    <pageSetUpPr/>
+  </sheetPr>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I23" sqref="I23"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="12.59765625" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.0"/>
   <cols>
-    <col min="1" max="1" width="4.8984375" customWidth="1"/>
-    <col min="2" max="2" width="32.8984375" customWidth="1"/>
-    <col min="3" max="3" width="33" customWidth="1"/>
-    <col min="4" max="4" width="21.3984375" customWidth="1"/>
-    <col min="5" max="5" width="52.5" customWidth="1"/>
-    <col min="6" max="7" width="9.8984375" customWidth="1"/>
-    <col min="8" max="8" width="10.5" customWidth="1"/>
-    <col min="9" max="26" width="9.3984375" customWidth="1"/>
+    <col customWidth="1" min="1" max="1" width="4.88"/>
+    <col customWidth="1" min="2" max="2" width="32.88"/>
+    <col customWidth="1" min="3" max="3" width="33.0"/>
+    <col customWidth="1" min="4" max="4" width="21.38"/>
+    <col customWidth="1" min="5" max="5" width="52.5"/>
+    <col customWidth="1" min="6" max="7" width="9.88"/>
+    <col customWidth="1" min="8" max="8" width="10.5"/>
+    <col customWidth="1" min="9" max="26" width="9.38"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="14.4">
-      <c r="B1" s="30" t="s">
+    <row r="1">
+      <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="31"/>
-      <c r="D1" s="31"/>
-      <c r="E1" s="31"/>
-      <c r="F1" s="31"/>
-      <c r="G1" s="31"/>
-      <c r="H1" s="31"/>
-    </row>
-    <row r="2" spans="1:8" ht="14.4">
-      <c r="B2" s="1" t="s">
+    </row>
+    <row r="2">
+      <c r="B2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="32" t="s">
+      <c r="C2" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="31"/>
-    </row>
-    <row r="3" spans="1:8" ht="14.4">
-      <c r="B3" s="2" t="s">
+    </row>
+    <row r="3">
+      <c r="B3" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="C3" s="3">
+      <c r="C3" s="5">
+        <v>5.0</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="B4" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C4" s="6" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="4" spans="1:8" ht="28.8">
-      <c r="B4" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C4" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="D4" s="5" t="s">
+      <c r="D4" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="E4" s="6"/>
-    </row>
-    <row r="5" spans="1:8" ht="14.4">
-      <c r="B5" s="2" t="s">
+      <c r="E4" s="8"/>
+    </row>
+    <row r="5">
+      <c r="B5" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="C5" s="7" t="s">
+      <c r="C5" s="9" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="1:8" ht="14.4">
-      <c r="B6" s="2" t="s">
+    <row r="6">
+      <c r="B6" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="C6" s="8">
-        <v>44480</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" ht="14.4">
-      <c r="B7" s="2" t="s">
+      <c r="C6" s="10">
+        <v>44480.0</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="B7" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="C7" s="8">
-        <v>44550</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" ht="14.4">
-      <c r="B8" s="9"/>
-      <c r="C8" s="9"/>
-      <c r="E8" s="9"/>
-      <c r="F8" s="9"/>
-      <c r="G8" s="9"/>
-      <c r="H8" s="9"/>
-    </row>
-    <row r="9" spans="1:8" ht="14.4">
-      <c r="B9" s="10" t="s">
+      <c r="C7" s="10">
+        <v>44550.0</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="B8" s="11"/>
+      <c r="C8" s="11"/>
+      <c r="E8" s="11"/>
+      <c r="F8" s="11"/>
+      <c r="G8" s="11"/>
+      <c r="H8" s="11"/>
+    </row>
+    <row r="9">
+      <c r="B9" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="C9" s="10" t="s">
+      <c r="C9" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="D9" s="10" t="s">
+      <c r="D9" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="E9" s="10" t="s">
+      <c r="E9" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="F9" s="10" t="s">
+      <c r="F9" s="12" t="s">
         <v>15</v>
       </c>
-      <c r="G9" s="10" t="s">
+      <c r="G9" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="H9" s="10" t="s">
+      <c r="H9" s="12" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="10" spans="1:8" ht="19.5" customHeight="1">
-      <c r="B10" s="11" t="s">
+    <row r="10" ht="19.5" customHeight="1">
+      <c r="B10" s="13" t="s">
         <v>18</v>
       </c>
-      <c r="C10" s="11" t="s">
+      <c r="C10" s="13" t="s">
         <v>19</v>
       </c>
-      <c r="D10" s="11" t="s">
+      <c r="D10" s="13" t="s">
         <v>19</v>
       </c>
-      <c r="E10" s="12" t="s">
+      <c r="E10" s="14" t="s">
         <v>20</v>
       </c>
-      <c r="F10" s="13">
-        <v>44480</v>
-      </c>
-      <c r="G10" s="13">
-        <v>44487</v>
-      </c>
-      <c r="H10" s="14">
+      <c r="F10" s="15">
+        <v>44480.0</v>
+      </c>
+      <c r="G10" s="15">
+        <v>44487.0</v>
+      </c>
+      <c r="H10" s="16">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="11" ht="19.5" customHeight="1">
+      <c r="B11" s="14" t="s">
+        <v>21</v>
+      </c>
+      <c r="C11" s="14" t="s">
+        <v>22</v>
+      </c>
+      <c r="D11" s="14" t="s">
+        <v>23</v>
+      </c>
+      <c r="E11" s="14" t="s">
+        <v>24</v>
+      </c>
+      <c r="F11" s="15">
+        <v>44480.0</v>
+      </c>
+      <c r="G11" s="15">
+        <v>44487.0</v>
+      </c>
+      <c r="H11" s="16">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="12" ht="19.5" customHeight="1">
+      <c r="B12" s="13" t="s">
+        <v>25</v>
+      </c>
+      <c r="C12" s="13" t="s">
+        <v>26</v>
+      </c>
+      <c r="D12" s="14" t="s">
+        <v>27</v>
+      </c>
+      <c r="E12" s="14" t="s">
+        <v>28</v>
+      </c>
+      <c r="F12" s="15">
+        <v>44480.0</v>
+      </c>
+      <c r="G12" s="15">
+        <v>44487.0</v>
+      </c>
+      <c r="H12" s="16">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="13" ht="19.5" customHeight="1">
+      <c r="A13" s="2"/>
+      <c r="B13" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="C13" s="14" t="s">
+        <v>30</v>
+      </c>
+      <c r="D13" s="14" t="s">
+        <v>31</v>
+      </c>
+      <c r="E13" s="14" t="s">
+        <v>24</v>
+      </c>
+      <c r="F13" s="15">
+        <v>44480.0</v>
+      </c>
+      <c r="G13" s="15">
+        <v>44487.0</v>
+      </c>
+      <c r="H13" s="16">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="14" ht="19.5" customHeight="1">
+      <c r="A14" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="B14" s="13" t="s">
+        <v>33</v>
+      </c>
+      <c r="C14" s="13" t="s">
+        <v>34</v>
+      </c>
+      <c r="D14" s="14" t="s">
+        <v>35</v>
+      </c>
+      <c r="E14" s="14" t="s">
+        <v>36</v>
+      </c>
+      <c r="F14" s="15">
+        <v>44487.0</v>
+      </c>
+      <c r="G14" s="15">
+        <v>44494.0</v>
+      </c>
+      <c r="H14" s="16">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="15" ht="19.5" customHeight="1">
+      <c r="B15" s="13" t="s">
+        <v>37</v>
+      </c>
+      <c r="C15" s="13" t="s">
+        <v>38</v>
+      </c>
+      <c r="D15" s="14" t="s">
+        <v>39</v>
+      </c>
+      <c r="E15" s="14" t="s">
+        <v>40</v>
+      </c>
+      <c r="F15" s="15">
+        <v>44487.0</v>
+      </c>
+      <c r="G15" s="15">
+        <v>44494.0</v>
+      </c>
+      <c r="H15" s="16">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="16" ht="19.5" customHeight="1">
+      <c r="B16" s="13" t="s">
+        <v>41</v>
+      </c>
+      <c r="C16" s="13" t="s">
+        <v>42</v>
+      </c>
+      <c r="D16" s="14" t="s">
+        <v>43</v>
+      </c>
+      <c r="E16" s="14" t="s">
+        <v>44</v>
+      </c>
+      <c r="F16" s="15">
+        <v>44487.0</v>
+      </c>
+      <c r="G16" s="15">
+        <v>44494.0</v>
+      </c>
+      <c r="H16" s="16">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="17" ht="19.5" customHeight="1">
+      <c r="B17" s="13" t="s">
+        <v>45</v>
+      </c>
+      <c r="C17" s="13" t="s">
+        <v>46</v>
+      </c>
+      <c r="D17" s="14" t="s">
+        <v>47</v>
+      </c>
+      <c r="E17" s="14" t="s">
+        <v>48</v>
+      </c>
+      <c r="F17" s="15">
+        <v>44487.0</v>
+      </c>
+      <c r="G17" s="15">
+        <v>44494.0</v>
+      </c>
+      <c r="H17" s="16">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="18" ht="19.5" customHeight="1">
+      <c r="B18" s="14" t="s">
+        <v>49</v>
+      </c>
+      <c r="C18" s="13" t="s">
+        <v>50</v>
+      </c>
+      <c r="D18" s="14" t="s">
+        <v>51</v>
+      </c>
+      <c r="E18" s="14" t="s">
+        <v>52</v>
+      </c>
+      <c r="F18" s="15">
+        <v>44493.0</v>
+      </c>
+      <c r="G18" s="15">
+        <v>44500.0</v>
+      </c>
+      <c r="H18" s="16">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="19" ht="19.5" customHeight="1">
+      <c r="B19" s="13" t="s">
+        <v>53</v>
+      </c>
+      <c r="C19" s="13" t="s">
+        <v>19</v>
+      </c>
+      <c r="D19" s="13" t="s">
+        <v>19</v>
+      </c>
+      <c r="E19" s="13"/>
+      <c r="F19" s="15">
+        <v>44501.0</v>
+      </c>
+      <c r="G19" s="17">
+        <v>44501.0</v>
+      </c>
+      <c r="H19" s="16">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="20" ht="19.5" customHeight="1">
+      <c r="B20" s="18" t="s">
+        <v>54</v>
+      </c>
+      <c r="C20" s="19"/>
+      <c r="D20" s="19"/>
+      <c r="E20" s="19"/>
+      <c r="F20" s="20">
+        <v>44480.0</v>
+      </c>
+      <c r="G20" s="20">
+        <v>44501.0</v>
+      </c>
+      <c r="H20" s="21">
+        <f>(H10+H11+H12+H14+H15+H16+H17+H18+H19)/9</f>
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:8" ht="19.5" customHeight="1">
-      <c r="B11" s="12" t="s">
-        <v>21</v>
-      </c>
-      <c r="C11" s="12" t="s">
-        <v>22</v>
-      </c>
-      <c r="D11" s="12" t="s">
-        <v>23</v>
-      </c>
-      <c r="E11" s="12" t="s">
-        <v>24</v>
-      </c>
-      <c r="F11" s="13">
-        <v>44480</v>
-      </c>
-      <c r="G11" s="13">
-        <v>44487</v>
-      </c>
-      <c r="H11" s="14">
+    <row r="21" ht="19.5" customHeight="1">
+      <c r="B21" s="13" t="s">
+        <v>55</v>
+      </c>
+      <c r="C21" s="13" t="s">
+        <v>56</v>
+      </c>
+      <c r="D21" s="14" t="s">
+        <v>57</v>
+      </c>
+      <c r="E21" s="14" t="s">
+        <v>58</v>
+      </c>
+      <c r="F21" s="17">
+        <v>44501.0</v>
+      </c>
+      <c r="G21" s="17">
+        <v>44514.0</v>
+      </c>
+      <c r="H21" s="16">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="22" ht="19.5" customHeight="1">
+      <c r="B22" s="22" t="s">
+        <v>59</v>
+      </c>
+      <c r="C22" s="14" t="s">
+        <v>60</v>
+      </c>
+      <c r="D22" s="14" t="s">
+        <v>61</v>
+      </c>
+      <c r="E22" s="14" t="s">
+        <v>62</v>
+      </c>
+      <c r="F22" s="17">
+        <v>44501.0</v>
+      </c>
+      <c r="G22" s="17">
+        <v>44521.0</v>
+      </c>
+      <c r="H22" s="16">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="23" ht="19.5" customHeight="1">
+      <c r="B23" s="13" t="s">
+        <v>53</v>
+      </c>
+      <c r="C23" s="13" t="s">
+        <v>19</v>
+      </c>
+      <c r="D23" s="13" t="s">
+        <v>19</v>
+      </c>
+      <c r="E23" s="13"/>
+      <c r="F23" s="17">
+        <v>44521.0</v>
+      </c>
+      <c r="G23" s="17">
+        <v>44521.0</v>
+      </c>
+      <c r="H23" s="16">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="24" ht="19.5" customHeight="1">
+      <c r="B24" s="18" t="s">
+        <v>63</v>
+      </c>
+      <c r="C24" s="19"/>
+      <c r="D24" s="19"/>
+      <c r="E24" s="19"/>
+      <c r="F24" s="23">
+        <v>44501.0</v>
+      </c>
+      <c r="G24" s="23">
+        <v>44521.0</v>
+      </c>
+      <c r="H24" s="21">
+        <f>(H21+H22+H23)/3</f>
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:8" ht="19.5" customHeight="1">
-      <c r="B12" s="11" t="s">
-        <v>25</v>
-      </c>
-      <c r="C12" s="11" t="s">
-        <v>26</v>
-      </c>
-      <c r="D12" s="12" t="s">
-        <v>27</v>
-      </c>
-      <c r="E12" s="12" t="s">
-        <v>28</v>
-      </c>
-      <c r="F12" s="13">
-        <v>44480</v>
-      </c>
-      <c r="G12" s="13">
-        <v>44487</v>
-      </c>
-      <c r="H12" s="14">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" ht="19.5" customHeight="1">
-      <c r="A13" s="1"/>
-      <c r="B13" s="15" t="s">
-        <v>29</v>
-      </c>
-      <c r="C13" s="15" t="s">
-        <v>30</v>
-      </c>
-      <c r="D13" s="12" t="s">
-        <v>31</v>
-      </c>
-      <c r="E13" s="12" t="s">
-        <v>24</v>
-      </c>
-      <c r="F13" s="13">
-        <v>44480</v>
-      </c>
-      <c r="G13" s="13">
-        <v>44487</v>
-      </c>
-      <c r="H13" s="14">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" ht="19.5" customHeight="1">
-      <c r="A14" s="1" t="s">
+    <row r="25" ht="19.5" customHeight="1">
+      <c r="B25" s="14" t="s">
+        <v>64</v>
+      </c>
+      <c r="C25" s="14" t="s">
+        <v>65</v>
+      </c>
+      <c r="D25" s="14" t="s">
+        <v>66</v>
+      </c>
+      <c r="E25" s="14" t="s">
+        <v>67</v>
+      </c>
+      <c r="F25" s="17">
+        <v>44522.0</v>
+      </c>
+      <c r="G25" s="17">
+        <v>44542.0</v>
+      </c>
+      <c r="H25" s="16">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="26" ht="19.5" customHeight="1">
+      <c r="B26" s="13" t="s">
+        <v>68</v>
+      </c>
+      <c r="C26" s="13" t="s">
+        <v>69</v>
+      </c>
+      <c r="D26" s="14" t="s">
+        <v>70</v>
+      </c>
+      <c r="E26" s="14" t="s">
+        <v>71</v>
+      </c>
+      <c r="F26" s="17">
+        <v>44522.0</v>
+      </c>
+      <c r="G26" s="17">
+        <v>44542.0</v>
+      </c>
+      <c r="H26" s="16">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="27" ht="19.5" customHeight="1">
+      <c r="A27" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="B14" s="11" t="s">
-        <v>33</v>
-      </c>
-      <c r="C14" s="11" t="s">
-        <v>34</v>
-      </c>
-      <c r="D14" s="12" t="s">
-        <v>35</v>
-      </c>
-      <c r="E14" s="12" t="s">
-        <v>36</v>
-      </c>
-      <c r="F14" s="13">
-        <v>44487</v>
-      </c>
-      <c r="G14" s="13">
-        <v>44494</v>
-      </c>
-      <c r="H14" s="14">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" ht="19.5" customHeight="1">
-      <c r="B15" s="11" t="s">
-        <v>37</v>
-      </c>
-      <c r="C15" s="11" t="s">
-        <v>38</v>
-      </c>
-      <c r="D15" s="12" t="s">
-        <v>39</v>
-      </c>
-      <c r="E15" s="12" t="s">
-        <v>40</v>
-      </c>
-      <c r="F15" s="13">
-        <v>44487</v>
-      </c>
-      <c r="G15" s="13">
-        <v>44494</v>
-      </c>
-      <c r="H15" s="14">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8" ht="19.5" customHeight="1">
-      <c r="B16" s="11" t="s">
-        <v>41</v>
-      </c>
-      <c r="C16" s="11" t="s">
-        <v>42</v>
-      </c>
-      <c r="D16" s="12" t="s">
-        <v>43</v>
-      </c>
-      <c r="E16" s="12" t="s">
-        <v>44</v>
-      </c>
-      <c r="F16" s="13">
-        <v>44487</v>
-      </c>
-      <c r="G16" s="13">
-        <v>44494</v>
-      </c>
-      <c r="H16" s="14">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8" ht="19.5" customHeight="1">
-      <c r="B17" s="11" t="s">
-        <v>45</v>
-      </c>
-      <c r="C17" s="11" t="s">
-        <v>46</v>
-      </c>
-      <c r="D17" s="12" t="s">
-        <v>47</v>
-      </c>
-      <c r="E17" s="12" t="s">
-        <v>48</v>
-      </c>
-      <c r="F17" s="13">
-        <v>44487</v>
-      </c>
-      <c r="G17" s="13">
-        <v>44494</v>
-      </c>
-      <c r="H17" s="14">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="18" spans="1:8" ht="19.5" customHeight="1">
-      <c r="B18" s="12" t="s">
-        <v>49</v>
-      </c>
-      <c r="C18" s="11" t="s">
-        <v>50</v>
-      </c>
-      <c r="D18" s="12" t="s">
-        <v>51</v>
-      </c>
-      <c r="E18" s="12" t="s">
-        <v>52</v>
-      </c>
-      <c r="F18" s="13">
-        <v>44493</v>
-      </c>
-      <c r="G18" s="13">
-        <v>44500</v>
-      </c>
-      <c r="H18" s="14">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="19" spans="1:8" ht="19.5" customHeight="1">
-      <c r="B19" s="11" t="s">
+      <c r="B27" s="13" t="s">
+        <v>72</v>
+      </c>
+      <c r="C27" s="13" t="s">
+        <v>73</v>
+      </c>
+      <c r="D27" s="14" t="s">
+        <v>74</v>
+      </c>
+      <c r="E27" s="14" t="s">
+        <v>75</v>
+      </c>
+      <c r="F27" s="17">
+        <v>44542.0</v>
+      </c>
+      <c r="G27" s="17">
+        <v>44549.0</v>
+      </c>
+      <c r="H27" s="16">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="28" ht="19.5" customHeight="1">
+      <c r="A28" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="B28" s="13" t="s">
+        <v>76</v>
+      </c>
+      <c r="C28" s="13" t="s">
+        <v>77</v>
+      </c>
+      <c r="D28" s="14" t="s">
+        <v>78</v>
+      </c>
+      <c r="E28" s="14" t="s">
+        <v>79</v>
+      </c>
+      <c r="F28" s="17">
+        <v>44542.0</v>
+      </c>
+      <c r="G28" s="17">
+        <v>44549.0</v>
+      </c>
+      <c r="H28" s="16">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="29" ht="19.5" customHeight="1">
+      <c r="B29" s="13" t="s">
         <v>53</v>
       </c>
-      <c r="C19" s="11" t="s">
+      <c r="C29" s="13" t="s">
         <v>19</v>
       </c>
-      <c r="D19" s="11" t="s">
+      <c r="D29" s="13" t="s">
         <v>19</v>
       </c>
-      <c r="E19" s="11"/>
-      <c r="F19" s="13">
-        <v>44501</v>
-      </c>
-      <c r="G19" s="16">
-        <v>44501</v>
-      </c>
-      <c r="H19" s="14"/>
-    </row>
-    <row r="20" spans="1:8" ht="19.5" customHeight="1">
-      <c r="B20" s="17" t="s">
-        <v>54</v>
-      </c>
-      <c r="C20" s="18"/>
-      <c r="D20" s="18"/>
-      <c r="E20" s="18"/>
-      <c r="F20" s="19">
-        <v>44480</v>
-      </c>
-      <c r="G20" s="19">
-        <v>44501</v>
-      </c>
-      <c r="H20" s="20">
-        <f>(H10+H11+H12+H14+H15+H16+H17+H18)/8</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="21" spans="1:8" ht="19.5" customHeight="1">
-      <c r="B21" s="11" t="s">
-        <v>55</v>
-      </c>
-      <c r="C21" s="11" t="s">
-        <v>56</v>
-      </c>
-      <c r="D21" s="12" t="s">
-        <v>57</v>
-      </c>
-      <c r="E21" s="12" t="s">
-        <v>58</v>
-      </c>
-      <c r="F21" s="16">
-        <v>44501</v>
-      </c>
-      <c r="G21" s="16">
-        <v>44514</v>
-      </c>
-      <c r="H21" s="14">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="22" spans="1:8" ht="19.5" customHeight="1">
-      <c r="B22" s="21" t="s">
-        <v>59</v>
-      </c>
-      <c r="C22" s="12" t="s">
-        <v>60</v>
-      </c>
-      <c r="D22" s="12" t="s">
-        <v>61</v>
-      </c>
-      <c r="E22" s="12" t="s">
-        <v>62</v>
-      </c>
-      <c r="F22" s="16">
-        <v>44501</v>
-      </c>
-      <c r="G22" s="16">
-        <v>44521</v>
-      </c>
-      <c r="H22" s="14">
-        <v>0.8</v>
-      </c>
-    </row>
-    <row r="23" spans="1:8" ht="19.5" customHeight="1">
-      <c r="B23" s="11" t="s">
-        <v>53</v>
-      </c>
-      <c r="C23" s="11" t="s">
-        <v>19</v>
-      </c>
-      <c r="D23" s="11" t="s">
-        <v>19</v>
-      </c>
-      <c r="E23" s="11"/>
-      <c r="F23" s="16">
-        <v>44521</v>
-      </c>
-      <c r="G23" s="16">
-        <v>44521</v>
-      </c>
-      <c r="H23" s="14"/>
-    </row>
-    <row r="24" spans="1:8" ht="19.5" customHeight="1">
-      <c r="B24" s="17" t="s">
-        <v>63</v>
-      </c>
-      <c r="C24" s="18"/>
-      <c r="D24" s="18"/>
-      <c r="E24" s="18"/>
-      <c r="F24" s="22">
-        <v>44501</v>
-      </c>
-      <c r="G24" s="22">
-        <v>44521</v>
-      </c>
-      <c r="H24" s="20">
-        <f>(H21+H22)/2</f>
-        <v>0.9</v>
-      </c>
-    </row>
-    <row r="25" spans="1:8" ht="19.5" customHeight="1">
-      <c r="B25" s="12" t="s">
-        <v>64</v>
-      </c>
-      <c r="C25" s="12" t="s">
-        <v>65</v>
-      </c>
-      <c r="D25" s="12" t="s">
-        <v>66</v>
-      </c>
-      <c r="E25" s="12" t="s">
-        <v>67</v>
-      </c>
-      <c r="F25" s="16">
-        <v>44522</v>
-      </c>
-      <c r="G25" s="16">
-        <v>44542</v>
-      </c>
-      <c r="H25" s="14">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="26" spans="1:8" ht="19.5" customHeight="1">
-      <c r="B26" s="11" t="s">
-        <v>68</v>
-      </c>
-      <c r="C26" s="11" t="s">
-        <v>69</v>
-      </c>
-      <c r="D26" s="12" t="s">
-        <v>70</v>
-      </c>
-      <c r="E26" s="12" t="s">
-        <v>71</v>
-      </c>
-      <c r="F26" s="16">
-        <v>44522</v>
-      </c>
-      <c r="G26" s="16">
-        <v>44542</v>
-      </c>
-      <c r="H26" s="14">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="27" spans="1:8" ht="19.5" customHeight="1">
-      <c r="A27" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="B27" s="11" t="s">
-        <v>72</v>
-      </c>
-      <c r="C27" s="11" t="s">
-        <v>73</v>
-      </c>
-      <c r="D27" s="12" t="s">
-        <v>74</v>
-      </c>
-      <c r="E27" s="12" t="s">
-        <v>75</v>
-      </c>
-      <c r="F27" s="16">
-        <v>44542</v>
-      </c>
-      <c r="G27" s="16">
-        <v>44549</v>
-      </c>
-      <c r="H27" s="14">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="28" spans="1:8" ht="19.5" customHeight="1">
-      <c r="A28" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="B28" s="11" t="s">
-        <v>76</v>
-      </c>
-      <c r="C28" s="11" t="s">
-        <v>77</v>
-      </c>
-      <c r="D28" s="12" t="s">
-        <v>78</v>
-      </c>
-      <c r="E28" s="12" t="s">
-        <v>79</v>
-      </c>
-      <c r="F28" s="16">
-        <v>44542</v>
-      </c>
-      <c r="G28" s="16">
-        <v>44549</v>
-      </c>
-      <c r="H28" s="14">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="29" spans="1:8" ht="19.5" customHeight="1">
-      <c r="B29" s="11" t="s">
-        <v>53</v>
-      </c>
-      <c r="C29" s="11" t="s">
-        <v>19</v>
-      </c>
-      <c r="D29" s="11" t="s">
-        <v>19</v>
-      </c>
-      <c r="E29" s="11"/>
-      <c r="F29" s="16">
-        <v>44549</v>
-      </c>
-      <c r="G29" s="16">
-        <v>44549</v>
-      </c>
-      <c r="H29" s="14">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="30" spans="1:8" ht="19.5" customHeight="1">
-      <c r="B30" s="17" t="s">
+      <c r="E29" s="13"/>
+      <c r="F29" s="17">
+        <v>44549.0</v>
+      </c>
+      <c r="G29" s="17">
+        <v>44549.0</v>
+      </c>
+      <c r="H29" s="16">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="30" ht="19.5" customHeight="1">
+      <c r="B30" s="18" t="s">
         <v>80</v>
       </c>
-      <c r="C30" s="18"/>
-      <c r="D30" s="18"/>
-      <c r="E30" s="18"/>
-      <c r="F30" s="23">
-        <v>44522</v>
-      </c>
-      <c r="G30" s="22">
-        <v>44549</v>
-      </c>
-      <c r="H30" s="20">
+      <c r="C30" s="19"/>
+      <c r="D30" s="19"/>
+      <c r="E30" s="19"/>
+      <c r="F30" s="24">
+        <v>44522.0</v>
+      </c>
+      <c r="G30" s="23">
+        <v>44549.0</v>
+      </c>
+      <c r="H30" s="21">
         <f>(H25+ H26+H27+H28+H29)/5</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="31" spans="1:8" ht="15.75" customHeight="1"/>
-    <row r="32" spans="1:8" ht="15.75" customHeight="1"/>
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="31" ht="15.75" customHeight="1"/>
+    <row r="32" ht="15.75" customHeight="1"/>
     <row r="33" ht="15.75" customHeight="1"/>
     <row r="34" ht="15.75" customHeight="1"/>
     <row r="35" ht="15.75" customHeight="1"/>
@@ -2282,135 +2272,139 @@
     <mergeCell ref="C2:D2"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="C2" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink r:id="rId1" ref="C2"/>
   </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
+  <printOptions/>
+  <pageMargins bottom="0.75" footer="0.0" header="0.0" left="0.7" right="0.7" top="0.75"/>
   <pageSetup paperSize="9" orientation="portrait"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
+    <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="B2:D12"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="12.59765625" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.0"/>
   <cols>
-    <col min="2" max="2" width="22.09765625" customWidth="1"/>
-    <col min="3" max="3" width="23.69921875" customWidth="1"/>
-    <col min="4" max="4" width="15.69921875" customWidth="1"/>
+    <col customWidth="1" min="2" max="2" width="22.13"/>
+    <col customWidth="1" min="3" max="3" width="23.75"/>
+    <col customWidth="1" min="4" max="4" width="15.75"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:4" ht="15" customHeight="1">
-      <c r="B2" s="1" t="s">
+    <row r="2" ht="15.0" customHeight="1">
+      <c r="B2" s="2" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="4" spans="2:4" ht="18" customHeight="1">
-      <c r="B4" s="24" t="s">
+    <row r="4" ht="18.0" customHeight="1">
+      <c r="B4" s="25" t="s">
         <v>82</v>
       </c>
-      <c r="C4" s="24" t="s">
+      <c r="C4" s="25" t="s">
         <v>83</v>
       </c>
-      <c r="D4" s="24" t="s">
+      <c r="D4" s="25" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="5" spans="2:4" ht="15" customHeight="1">
-      <c r="B5" s="25" t="s">
+    <row r="5" ht="15.0" customHeight="1">
+      <c r="B5" s="26" t="s">
         <v>85</v>
       </c>
-      <c r="C5" s="11" t="s">
+      <c r="C5" s="13" t="s">
         <v>86</v>
       </c>
-      <c r="D5" s="12" t="s">
+      <c r="D5" s="14" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="6" spans="2:4" ht="15" customHeight="1">
-      <c r="B6" s="26" t="s">
+    <row r="6" ht="15.0" customHeight="1">
+      <c r="B6" s="27" t="s">
         <v>88</v>
       </c>
-      <c r="C6" s="11" t="s">
+      <c r="C6" s="13" t="s">
         <v>89</v>
       </c>
-      <c r="D6" s="11" t="s">
+      <c r="D6" s="13" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="7" spans="2:4" ht="15" customHeight="1">
-      <c r="B7" s="26" t="s">
+    <row r="7" ht="15.0" customHeight="1">
+      <c r="B7" s="27" t="s">
         <v>91</v>
       </c>
-      <c r="C7" s="11" t="s">
+      <c r="C7" s="13" t="s">
         <v>92</v>
       </c>
-      <c r="D7" s="11" t="s">
+      <c r="D7" s="13" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="8" spans="2:4" ht="15" customHeight="1">
-      <c r="B8" s="26" t="s">
+    <row r="8" ht="15.0" customHeight="1">
+      <c r="B8" s="27" t="s">
         <v>94</v>
       </c>
-      <c r="C8" s="12" t="s">
+      <c r="C8" s="14" t="s">
         <v>89</v>
       </c>
-      <c r="D8" s="12" t="s">
+      <c r="D8" s="14" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="9" spans="2:4" ht="15" customHeight="1">
-      <c r="B9" s="26" t="s">
+    <row r="9" ht="15.0" customHeight="1">
+      <c r="B9" s="27" t="s">
         <v>95</v>
       </c>
-      <c r="C9" s="11" t="s">
+      <c r="C9" s="13" t="s">
         <v>92</v>
       </c>
-      <c r="D9" s="11" t="s">
+      <c r="D9" s="13" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="10" spans="2:4" ht="15" customHeight="1">
-      <c r="B10" s="27" t="s">
+    <row r="10" ht="15.0" customHeight="1">
+      <c r="B10" s="28" t="s">
         <v>96</v>
       </c>
-      <c r="C10" s="28" t="s">
+      <c r="C10" s="29" t="s">
         <v>97</v>
       </c>
-      <c r="D10" s="28" t="s">
+      <c r="D10" s="29" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="11" spans="2:4" ht="14.4">
-      <c r="B11" s="29" t="s">
+    <row r="11">
+      <c r="B11" s="30" t="s">
         <v>99</v>
       </c>
-      <c r="C11" s="29" t="s">
+      <c r="C11" s="30" t="s">
         <v>100</v>
       </c>
-      <c r="D11" s="29" t="s">
+      <c r="D11" s="30" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="12" spans="2:4" ht="14.4">
-      <c r="B12" s="21" t="s">
+    <row r="12">
+      <c r="B12" s="22" t="s">
         <v>102</v>
       </c>
-      <c r="C12" s="21" t="s">
+      <c r="C12" s="22" t="s">
         <v>103</v>
       </c>
-      <c r="D12" s="21" t="s">
+      <c r="D12" s="22" t="s">
         <v>104</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
+  <printOptions/>
+  <pageMargins bottom="0.75" footer="0.0" header="0.0" left="0.7" right="0.7" top="0.75"/>
   <pageSetup orientation="landscape"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>